<commit_message>
worked on paper SI part
</commit_message>
<xml_diff>
--- a/Youngs_Moduli.xlsx
+++ b/Youngs_Moduli.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_RESEARCH\08_Dynamic Mechanical Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F882EB4-6CCA-4540-9E51-1F38A365F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889AF672-A81F-4F56-9C32-8E0615F7C596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{119970A3-6474-4D1D-A380-FC6377674E8E}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>gel</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Wasser1.2.CSV</t>
+  </si>
+  <si>
+    <t>STD/MEAN</t>
   </si>
 </sst>
 </file>
@@ -740,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61275085-EC9D-4700-9854-A34AB91270FB}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L2" sqref="L2:L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +763,7 @@
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,8 +794,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -823,8 +829,12 @@
       <c r="J2">
         <v>4552.8599999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>1.7700757567510658E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -855,8 +865,12 @@
       <c r="J3">
         <v>5244.46</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>1.7572334270464628E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -887,8 +901,12 @@
       <c r="J4">
         <v>11415.38</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>2.498923845756712E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -919,8 +937,12 @@
       <c r="J5">
         <v>2858.36</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>5.6026676158771127E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -951,8 +973,12 @@
       <c r="J6">
         <v>8129.78</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>2.258066299120555E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -983,8 +1009,12 @@
       <c r="J7">
         <v>4428.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>1.1311400595185759E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1015,8 +1045,12 @@
       <c r="J8">
         <v>3516.19</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>2.2798855709715442E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1047,24 +1081,36 @@
       <c r="J9">
         <v>3102.38</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>2.2608867639253606E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1095,8 +1141,12 @@
       <c r="J12">
         <v>5838.77</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>5.2908970784380345E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1127,8 +1177,12 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>5.8443439726034226E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1159,8 +1213,12 @@
       <c r="J14">
         <v>2663.89</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>3.3431099912289937E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1191,8 +1249,12 @@
       <c r="J15">
         <v>13315.26</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>3.410976906228786E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1223,24 +1285,36 @@
       <c r="J16">
         <v>3370.05</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>5.8874417158468932E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L17" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1271,8 +1345,12 @@
       <c r="J19">
         <v>8304.6299999999992</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>2.5521302355535232E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1303,8 +1381,12 @@
       <c r="J20">
         <v>2920.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>9.408764623148113E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1335,8 +1417,12 @@
       <c r="J21">
         <v>6982.76</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>3.8902574310203511E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -1367,8 +1453,12 @@
       <c r="J22">
         <v>6792.86</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>4.0270814209292079E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1399,8 +1489,12 @@
       <c r="J23">
         <v>9193.7000000000007</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>7.0415544926415122E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -1431,8 +1525,12 @@
       <c r="J24">
         <v>4997.28</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>3.8301862468378016E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1463,8 +1561,12 @@
       <c r="J25">
         <v>9831.89</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>1.9661111200765607E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -1495,8 +1597,12 @@
       <c r="J26">
         <v>8167.99</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>1.6002205674007439E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1527,8 +1633,12 @@
       <c r="J27">
         <v>7075.59</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>1.9410578818813751E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1559,8 +1669,12 @@
       <c r="J28">
         <v>7868.37</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>2.2182549114570835E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1591,8 +1705,12 @@
       <c r="J29">
         <v>7479.73</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.13380863350871602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
@@ -1623,8 +1741,12 @@
       <c r="J30">
         <v>5515.12</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>8.2753384524778581E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -1655,8 +1777,12 @@
       <c r="J31">
         <v>3896.07</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>5.2187376641558862E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -1687,8 +1813,12 @@
       <c r="J32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>6.0049537234153121E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -1719,24 +1849,36 @@
       <c r="J33">
         <v>6802.43</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>5.6316858588879144E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L34" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L35" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1767,8 +1909,12 @@
       <c r="J36">
         <v>9523.6200000000008</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>-1.5963559258110747</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -1799,8 +1945,12 @@
       <c r="J37">
         <v>6093.46</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>-1.867566921459614</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>63</v>
       </c>
@@ -1831,8 +1981,12 @@
       <c r="J38">
         <v>8671.82</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>-1.9873815155015311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -1863,8 +2017,12 @@
       <c r="J39">
         <v>14286.21</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.44837178092561708</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>66</v>
       </c>
@@ -1895,8 +2053,12 @@
       <c r="J40">
         <v>7615.31</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.24507220566304538</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>66</v>
       </c>
@@ -1927,8 +2089,12 @@
       <c r="J41">
         <v>7399.88</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.31925000916780094</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>69</v>
       </c>
@@ -1959,8 +2125,12 @@
       <c r="J42">
         <v>10301.61</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.39314290381105832</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>69</v>
       </c>
@@ -1991,24 +2161,36 @@
       <c r="J43">
         <v>6995.44</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>9.8797263113682018E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L44" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L45" t="e">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>75</v>
       </c>
@@ -2039,8 +2221,12 @@
       <c r="J46">
         <v>3299.99</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>1.9604045788298594E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>77</v>
       </c>
@@ -2071,8 +2257,12 @@
       <c r="J47">
         <v>8305.92</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>7.8710492514850044E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>77</v>
       </c>
@@ -2103,8 +2293,12 @@
       <c r="J48">
         <v>5176.2700000000004</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>7.814476256614257E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>80</v>
       </c>
@@ -2135,8 +2329,12 @@
       <c r="J49">
         <v>5982.65</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.51340571035290017</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>80</v>
       </c>
@@ -2167,8 +2365,12 @@
       <c r="J50">
         <v>3402.16</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>-0.27431531231530742</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>83</v>
       </c>
@@ -2199,8 +2401,12 @@
       <c r="J51">
         <v>5941.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>7.0933365615386781E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>83</v>
       </c>
@@ -2231,8 +2437,12 @@
       <c r="J52">
         <v>7171.46</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>6.3189257087915465E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>86</v>
       </c>
@@ -2263,8 +2473,12 @@
       <c r="J53">
         <v>15307.34</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.13821754345918313</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>86</v>
       </c>
@@ -2295,8 +2509,12 @@
       <c r="J54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>4.9452758333278217E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>86</v>
       </c>
@@ -2327,8 +2545,12 @@
       <c r="J55">
         <v>6426.47</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>8.3747817353452367E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>90</v>
       </c>
@@ -2359,8 +2581,12 @@
       <c r="J56">
         <v>8958.81</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>0.1537616186109225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>90</v>
       </c>
@@ -2391,8 +2617,12 @@
       <c r="J57">
         <v>2884.49</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>7.290325026537936E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>93</v>
       </c>
@@ -2423,8 +2653,12 @@
       <c r="J58">
         <v>4518.58</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>3.1542111446076021E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>93</v>
       </c>
@@ -2455,8 +2689,12 @@
       <c r="J59">
         <v>3593</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <f>youngs_moduli_korrigiert[[#This Row],[E_Std]]/youngs_moduli_korrigiert[[#This Row],[E_Mean_corrected]]</f>
+        <v>2.7538771186765447E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
@@ -2464,7 +2702,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>96</v>
       </c>

</xml_diff>